<commit_message>
@update ffan performance and stability test cases
</commit_message>
<xml_diff>
--- a/resources/templateStability.xlsx
+++ b/resources/templateStability.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="测试概述" sheetId="1" r:id="rId1"/>
@@ -428,34 +428,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -475,14 +472,14 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -819,169 +816,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="10"/>
     </row>
     <row r="3" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:20" s="1" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:20" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A3:T3"/>
     <mergeCell ref="A20:C20"/>
@@ -995,12 +998,6 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1024,67 +1021,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -1092,12 +1095,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,67 +1118,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -1189,12 +1192,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1218,67 +1215,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -1286,12 +1289,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1314,106 +1311,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="3"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-    </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="C9:E9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1435,64 +1438,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1530,64 +1533,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1628,67 +1631,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -1696,12 +1705,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1725,67 +1728,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -1793,12 +1802,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1822,67 +1825,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -1890,12 +1899,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1919,67 +1922,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -1987,12 +1996,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2016,67 +2019,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:B1"/>
@@ -2084,12 +2093,6 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>